<commit_message>
Glass panel size corrections left side and back
</commit_message>
<xml_diff>
--- a/cage-bom.xlsx
+++ b/cage-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/root/files/projs/ender5pro/enclosure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB532D7-13A1-6A44-9A40-82B7168E2000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B55AA1-666C-EA4C-90FC-EE4FA2415C26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="640" windowWidth="38420" windowHeight="25100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8960" yWindow="780" windowWidth="43660" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="222">
   <si>
     <t>Item</t>
   </si>
@@ -386,12 +386,6 @@
     <t>PS.B</t>
   </si>
   <si>
-    <t>PG.L</t>
-  </si>
-  <si>
-    <t>PX.R</t>
-  </si>
-  <si>
     <t>PS.T, PS.B</t>
   </si>
   <si>
@@ -422,9 +416,6 @@
     <t>Gasket Seal 3mm dia, for glass panel (meter)</t>
   </si>
   <si>
-    <t>PG.L, PS.K</t>
-  </si>
-  <si>
     <t>All glass panels</t>
   </si>
   <si>
@@ -696,6 +687,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FG.L</t>
+  </si>
+  <si>
+    <t>FX.R</t>
+  </si>
+  <si>
+    <t>FG.L, FX.R</t>
+  </si>
+  <si>
+    <t>Glass, tempered, 670 x 570 x 5mm, R=10mm</t>
+  </si>
+  <si>
+    <t>Gasket Seal for 670 x 570 glass panel</t>
   </si>
 </sst>
 </file>
@@ -2564,8 +2570,8 @@
   </sheetPr>
   <dimension ref="B1:L76"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2586,11 +2592,11 @@
     <row r="1" spans="2:11" ht="16" thickBot="1"/>
     <row r="2" spans="2:11" ht="18">
       <c r="B2" s="123" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C2" s="124"/>
       <c r="D2" s="125" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E2" s="125"/>
       <c r="F2" s="126"/>
@@ -2599,66 +2605,66 @@
     </row>
     <row r="3" spans="2:11" ht="18">
       <c r="B3" s="129" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="130"/>
       <c r="D3" s="127" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E3" s="127"/>
       <c r="F3" s="128"/>
     </row>
     <row r="4" spans="2:11" ht="18">
       <c r="B4" s="129" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="130"/>
       <c r="D4" s="131" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="131"/>
       <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:11" ht="18">
       <c r="B5" s="129" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" s="130"/>
       <c r="D5" s="131" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:11" ht="18">
       <c r="B6" s="129" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="130"/>
       <c r="D6" s="131" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:11" ht="19" thickBot="1">
       <c r="B7" s="118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C7" s="135"/>
       <c r="D7" s="133" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7" s="133"/>
       <c r="F7" s="134"/>
     </row>
     <row r="8" spans="2:11" ht="16" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
@@ -2679,7 +2685,7 @@
     </row>
     <row r="11" spans="2:11" ht="19" thickBot="1">
       <c r="B11" s="120" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
@@ -2693,7 +2699,7 @@
     </row>
     <row r="12" spans="2:11" s="3" customFormat="1" ht="16" thickBot="1">
       <c r="B12" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>1</v>
@@ -2731,16 +2737,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>62</v>
@@ -2754,16 +2760,16 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>63</v>
@@ -2783,13 +2789,13 @@
         <v>48</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
@@ -2803,19 +2809,19 @@
         <v>1</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
@@ -2835,10 +2841,10 @@
         <v>48</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>61</v>
@@ -2858,10 +2864,10 @@
         <v>48</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>64</v>
@@ -2881,10 +2887,10 @@
         <v>48</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>60</v>
@@ -2905,7 +2911,7 @@
         <v>68</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="2:11" s="3" customFormat="1">
@@ -2923,7 +2929,7 @@
         <v>73</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="2:11" s="3" customFormat="1">
@@ -2941,7 +2947,7 @@
         <v>74</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -2962,7 +2968,7 @@
     </row>
     <row r="27" spans="2:11" ht="16" thickBot="1">
       <c r="C27" s="114" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D27" s="115"/>
       <c r="E27" s="40"/>
@@ -3033,7 +3039,7 @@
     <row r="32" spans="2:11">
       <c r="B32" s="39"/>
       <c r="C32" s="116" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D32" s="117"/>
       <c r="E32" s="37"/>
@@ -3321,8 +3327,8 @@
   </sheetPr>
   <dimension ref="B1:J143"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3337,102 +3343,102 @@
     <col min="8" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="16" thickBot="1"/>
-    <row r="2" spans="2:9" ht="18">
+    <row r="1" spans="2:8" ht="16" thickBot="1"/>
+    <row r="2" spans="2:8" ht="18">
       <c r="B2" s="123" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C2" s="146"/>
       <c r="D2" s="139" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E2" s="125"/>
       <c r="F2" s="125"/>
       <c r="G2" s="126"/>
       <c r="H2" s="36"/>
     </row>
-    <row r="3" spans="2:9" ht="18">
+    <row r="3" spans="2:8" ht="18">
       <c r="B3" s="129" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="145"/>
       <c r="D3" s="140" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E3" s="127"/>
       <c r="F3" s="127"/>
       <c r="G3" s="128"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="2:9" ht="18">
+    <row r="4" spans="2:8" ht="18">
       <c r="B4" s="129" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="141" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="131"/>
       <c r="F4" s="131"/>
       <c r="G4" s="132"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:9" ht="18">
+    <row r="5" spans="2:8" ht="18">
       <c r="B5" s="129" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" s="145"/>
       <c r="D5" s="141" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="131"/>
       <c r="G5" s="132"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="2:9" ht="18">
+    <row r="6" spans="2:8" ht="18">
       <c r="B6" s="129" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="145"/>
       <c r="D6" s="141" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="131"/>
       <c r="G6" s="132"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="2:9" ht="19" thickBot="1">
+    <row r="7" spans="2:8" ht="19" thickBot="1">
       <c r="B7" s="118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C7" s="119"/>
       <c r="D7" s="142" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7" s="133"/>
       <c r="F7" s="133"/>
       <c r="G7" s="134"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="2:9" ht="16" thickBot="1">
+    <row r="8" spans="2:8" ht="16" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="143" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E8" s="144"/>
       <c r="F8" s="29"/>
       <c r="G8" s="17"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="10" spans="2:9" ht="16" thickBot="1"/>
-    <row r="11" spans="2:9" ht="19" thickBot="1">
+    <row r="10" spans="2:8" ht="16" thickBot="1"/>
+    <row r="11" spans="2:8" ht="19" thickBot="1">
       <c r="B11" s="136" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C11" s="137"/>
       <c r="D11" s="137"/>
@@ -3441,12 +3447,12 @@
       <c r="G11" s="138"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:9" s="3" customFormat="1" ht="16" thickBot="1">
+    <row r="12" spans="2:8" s="3" customFormat="1" ht="16" thickBot="1">
       <c r="B12" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>1</v>
@@ -3461,7 +3467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:9" s="3" customFormat="1">
+    <row r="13" spans="2:8" s="3" customFormat="1">
       <c r="B13" s="1">
         <v>207</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>66</v>
@@ -3480,12 +3486,8 @@
       <c r="G13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="3">
-        <f>IF(TRUNC(C13)=101,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" s="3" customFormat="1">
+    </row>
+    <row r="14" spans="2:8" s="3" customFormat="1">
       <c r="B14" s="1">
         <v>203</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>66</v>
@@ -3505,7 +3507,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="2:9" s="3" customFormat="1">
+    <row r="15" spans="2:8" s="3" customFormat="1">
       <c r="B15" s="1">
         <v>215</v>
       </c>
@@ -3516,16 +3518,16 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="2:9" s="3" customFormat="1">
+    <row r="16" spans="2:8" s="3" customFormat="1">
       <c r="B16" s="1">
         <v>211</v>
       </c>
@@ -3536,10 +3538,10 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>77</v>
@@ -3556,7 +3558,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>50</v>
@@ -3576,7 +3578,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>50</v>
@@ -3596,7 +3598,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>50</v>
@@ -3616,7 +3618,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>50</v>
@@ -3636,7 +3638,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>50</v>
@@ -3656,7 +3658,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>66</v>
@@ -3665,7 +3667,7 @@
         <v>79</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="2:10" s="3" customFormat="1">
@@ -3679,7 +3681,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>66</v>
@@ -3699,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>50</v>
@@ -3719,7 +3721,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -3739,7 +3741,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>50</v>
@@ -3759,7 +3761,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>50</v>
@@ -3779,7 +3781,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>50</v>
@@ -3802,10 +3804,10 @@
         <v>113</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>108</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="3" customFormat="1">
@@ -3816,16 +3818,16 @@
         <v>103.2</v>
       </c>
       <c r="D30" s="16">
-        <v>2.2799999999999998</v>
+        <v>2.48</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>113</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>77</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="2:10" s="3" customFormat="1">
@@ -4222,7 +4224,7 @@
         <v>101</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>102</v>
@@ -4242,7 +4244,7 @@
         <v>101</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>75</v>
@@ -4402,7 +4404,7 @@
         <v>103</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>102</v>
@@ -4422,7 +4424,7 @@
         <v>103</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>75</v>
@@ -4582,7 +4584,7 @@
         <v>86</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>105</v>
@@ -4602,7 +4604,7 @@
         <v>86</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>78</v>
@@ -4762,7 +4764,7 @@
         <v>88</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>107</v>
@@ -4782,7 +4784,7 @@
         <v>88</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>76</v>
@@ -5077,10 +5079,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:Q95"/>
+  <dimension ref="B2:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5115,11 +5117,11 @@
     </row>
     <row r="3" spans="2:17" ht="18">
       <c r="B3" s="123" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C3" s="146"/>
       <c r="D3" s="139" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E3" s="125"/>
       <c r="F3" s="125"/>
@@ -5132,11 +5134,11 @@
     </row>
     <row r="4" spans="2:17" ht="18">
       <c r="B4" s="129" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="140" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E4" s="127"/>
       <c r="F4" s="127"/>
@@ -5144,11 +5146,11 @@
     </row>
     <row r="5" spans="2:17" ht="18">
       <c r="B5" s="129" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="145"/>
       <c r="D5" s="141" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="131"/>
@@ -5156,11 +5158,11 @@
     </row>
     <row r="6" spans="2:17" ht="18">
       <c r="B6" s="129" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C6" s="145"/>
       <c r="D6" s="141" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="131"/>
@@ -5168,11 +5170,11 @@
     </row>
     <row r="7" spans="2:17" ht="18">
       <c r="B7" s="129" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C7" s="145"/>
       <c r="D7" s="141" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" s="131"/>
       <c r="F7" s="131"/>
@@ -5180,11 +5182,11 @@
     </row>
     <row r="8" spans="2:17" ht="19" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="142" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="133"/>
@@ -5192,11 +5194,11 @@
     </row>
     <row r="9" spans="2:17" ht="16" thickBot="1">
       <c r="B9" s="118" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C9" s="119"/>
       <c r="D9" s="143" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E9" s="144"/>
       <c r="F9" s="29"/>
@@ -5224,7 +5226,7 @@
     </row>
     <row r="12" spans="2:17" ht="19" thickBot="1">
       <c r="B12" s="120" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
@@ -5237,11 +5239,11 @@
       <c r="K12" s="121"/>
       <c r="L12" s="121"/>
       <c r="M12" s="108">
-        <f>SUM(M14:M32)</f>
-        <v>24.45232</v>
+        <f>SUM(M14:M33)</f>
+        <v>25.289820000000002</v>
       </c>
       <c r="Q12" s="112">
-        <f>SUM(Q14:Q32)</f>
+        <f>SUM(Q14:Q33)</f>
         <v>223.34</v>
       </c>
     </row>
@@ -5268,19 +5270,19 @@
         <v>9</v>
       </c>
       <c r="I13" s="110" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J13" s="110" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K13" s="110" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L13" s="110" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M13" s="106" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="2:17" s="3" customFormat="1">
@@ -5297,10 +5299,10 @@
         <v>66</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>82</v>
@@ -5342,10 +5344,10 @@
         <v>66</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>106</v>
@@ -5381,16 +5383,16 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>80</v>
@@ -5432,10 +5434,10 @@
         <v>66</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>104</v>
@@ -5471,16 +5473,16 @@
         <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>65</v>
@@ -5516,16 +5518,16 @@
         <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>81</v>
@@ -5561,16 +5563,16 @@
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>79</v>
@@ -5603,20 +5605,20 @@
         <v>211</v>
       </c>
       <c r="C21" s="7">
-        <v>12.16</v>
+        <v>12.36</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I21" s="111"/>
       <c r="J21" s="111"/>
@@ -5645,10 +5647,10 @@
         <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="7" t="s">
@@ -5693,10 +5695,10 @@
         <v>87</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="7" t="s">
@@ -5741,10 +5743,10 @@
         <v>88</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="7" t="s">
@@ -5783,16 +5785,16 @@
         <v>215</v>
       </c>
       <c r="C25" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>128</v>
+        <v>217</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="7" t="s">
@@ -5812,7 +5814,7 @@
       </c>
       <c r="M25" s="107">
         <f>C25*I25*J25*K25*L25/1000000000</f>
-        <v>7.8724999999999996</v>
+        <v>3.9362499999999998</v>
       </c>
       <c r="O25" s="3">
         <f>I25+J25</f>
@@ -5823,64 +5825,76 @@
       </c>
       <c r="Q25" s="113">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="2:17" s="3" customFormat="1">
       <c r="B26" s="1">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C26" s="7">
-        <v>180</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="111"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="105"/>
+        <v>220</v>
+      </c>
+      <c r="I26" s="111">
+        <v>670</v>
+      </c>
+      <c r="J26" s="111">
+        <v>570</v>
+      </c>
+      <c r="K26" s="111">
+        <v>5</v>
+      </c>
+      <c r="L26" s="111">
+        <v>2500</v>
+      </c>
+      <c r="M26" s="107">
+        <f>C26*I26*J26*K26*L26/1000000000</f>
+        <v>4.7737499999999997</v>
+      </c>
       <c r="O26" s="3">
-        <v>200</v>
+        <f>I26+J26</f>
+        <v>1240</v>
       </c>
       <c r="P26" s="109">
-        <v>0.1</v>
-      </c>
-      <c r="Q26" s="109">
-        <f>O26*P26</f>
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="Q26" s="113">
+        <f t="shared" ref="Q26" si="2">C26*P26</f>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:17" s="3" customFormat="1">
       <c r="B27" s="1">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="7">
         <v>180</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I27" s="111"/>
       <c r="J27" s="111"/>
@@ -5891,32 +5905,32 @@
         <v>200</v>
       </c>
       <c r="P27" s="109">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="Q27" s="109">
         <f>O27*P27</f>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:17" s="3" customFormat="1">
       <c r="B28" s="1">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="7">
         <v>180</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="7" t="s">
-        <v>70</v>
+        <v>211</v>
       </c>
       <c r="I28" s="111"/>
       <c r="J28" s="111"/>
@@ -5927,32 +5941,32 @@
         <v>200</v>
       </c>
       <c r="P28" s="109">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="Q28" s="109">
-        <f t="shared" ref="Q28:Q33" si="2">O28*P28</f>
-        <v>6</v>
+        <f>O28*P28</f>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:17" s="3" customFormat="1">
       <c r="B29" s="1">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="7">
         <v>180</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" s="111"/>
       <c r="J29" s="111"/>
@@ -5963,32 +5977,32 @@
         <v>200</v>
       </c>
       <c r="P29" s="109">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="Q29" s="109">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" ref="Q29:Q34" si="3">O29*P29</f>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:17" s="3" customFormat="1">
       <c r="B30" s="1">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" s="7">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="7" t="s">
-        <v>215</v>
+        <v>71</v>
       </c>
       <c r="I30" s="111"/>
       <c r="J30" s="111"/>
@@ -5996,35 +6010,35 @@
       <c r="L30" s="111"/>
       <c r="M30" s="105"/>
       <c r="O30" s="3">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="P30" s="109">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="Q30" s="109">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:17" s="3" customFormat="1">
       <c r="B31" s="1">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="7">
         <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="7" t="s">
-        <v>74</v>
+        <v>212</v>
       </c>
       <c r="I31" s="111"/>
       <c r="J31" s="111"/>
@@ -6035,112 +6049,135 @@
         <v>50</v>
       </c>
       <c r="P31" s="109">
-        <v>0.18</v>
+        <v>0.04</v>
       </c>
       <c r="Q31" s="109">
-        <f>O31*P31</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:17" s="3" customFormat="1">
       <c r="B32" s="1">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C32" s="7">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>208</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="G32" s="16"/>
       <c r="H32" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" s="111">
-        <v>10.725</v>
-      </c>
-      <c r="J32" s="111">
-        <v>10.725</v>
-      </c>
-      <c r="K32" s="111">
-        <v>10.725</v>
-      </c>
-      <c r="L32" s="111">
-        <v>2.7</v>
-      </c>
-      <c r="M32" s="107">
-        <f t="shared" ref="M32" si="3">C32*I32/1000*L32</f>
-        <v>1.04247</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="105"/>
       <c r="O32" s="3">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="P32" s="109">
-        <v>1.25</v>
+        <v>0.18</v>
       </c>
       <c r="Q32" s="109">
         <f>O32*P32</f>
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="2:17" s="3" customFormat="1">
       <c r="B33" s="1">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C33" s="7">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="111">
+        <v>10.725</v>
+      </c>
+      <c r="J33" s="111">
+        <v>10.725</v>
+      </c>
+      <c r="K33" s="111">
+        <v>10.725</v>
+      </c>
+      <c r="L33" s="111">
+        <v>2.7</v>
+      </c>
+      <c r="M33" s="107">
+        <f t="shared" ref="M33" si="4">C33*I33/1000*L33</f>
+        <v>1.04247</v>
+      </c>
+      <c r="O33" s="3">
+        <v>36</v>
+      </c>
+      <c r="P33" s="109">
+        <v>1.25</v>
+      </c>
+      <c r="Q33" s="109">
+        <f>O33*P33</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" s="3" customFormat="1">
+      <c r="B34" s="1">
+        <v>232</v>
+      </c>
+      <c r="C34" s="7">
+        <v>12</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="105"/>
-      <c r="O33" s="3">
-        <v>12</v>
-      </c>
-      <c r="P33" s="109">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="Q33" s="109">
-        <f t="shared" si="2"/>
-        <v>52.199999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="2:17" s="3" customFormat="1">
-      <c r="B34" s="1"/>
-      <c r="C34" s="7"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="105"/>
+      <c r="O34" s="3">
+        <v>12</v>
+      </c>
+      <c r="P34" s="109">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="Q34" s="109">
+        <f t="shared" si="3"/>
+        <v>52.199999999999996</v>
+      </c>
     </row>
     <row r="35" spans="2:17" s="3" customFormat="1">
       <c r="B35" s="1"/>
@@ -6284,6 +6321,9 @@
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
       <c r="M45" s="105"/>
+      <c r="O45" s="3">
+        <v>2480</v>
+      </c>
     </row>
     <row r="46" spans="2:17" s="3" customFormat="1">
       <c r="B46" s="1"/>
@@ -6297,87 +6337,112 @@
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
       <c r="M46" s="105"/>
-    </row>
-    <row r="47" spans="2:17">
-      <c r="G47" s="19"/>
+      <c r="O46" s="3">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" s="3" customFormat="1">
+      <c r="B47" s="1"/>
+      <c r="C47" s="7"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="105"/>
+      <c r="O47" s="3">
+        <v>1720</v>
+      </c>
     </row>
     <row r="48" spans="2:17">
       <c r="G48" s="19"/>
-    </row>
-    <row r="49" spans="7:7">
+      <c r="O48" s="6">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15">
       <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="7:7">
+      <c r="O49" s="6">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="50" spans="7:15">
       <c r="G50" s="19"/>
-    </row>
-    <row r="51" spans="7:7">
+      <c r="O50" s="6">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="51" spans="7:15">
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="7:7">
+    <row r="52" spans="7:15">
       <c r="G52" s="19"/>
     </row>
-    <row r="53" spans="7:7">
+    <row r="53" spans="7:15">
       <c r="G53" s="19"/>
     </row>
-    <row r="54" spans="7:7">
+    <row r="54" spans="7:15">
       <c r="G54" s="19"/>
     </row>
-    <row r="55" spans="7:7">
+    <row r="55" spans="7:15">
       <c r="G55" s="19"/>
     </row>
-    <row r="56" spans="7:7">
+    <row r="56" spans="7:15">
       <c r="G56" s="19"/>
     </row>
-    <row r="57" spans="7:7">
+    <row r="57" spans="7:15">
       <c r="G57" s="19"/>
     </row>
-    <row r="58" spans="7:7">
+    <row r="58" spans="7:15">
       <c r="G58" s="19"/>
     </row>
-    <row r="59" spans="7:7">
+    <row r="59" spans="7:15">
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="7:7">
+    <row r="60" spans="7:15">
       <c r="G60" s="19"/>
     </row>
-    <row r="61" spans="7:7">
-      <c r="G61" s="20"/>
-    </row>
-    <row r="62" spans="7:7">
+    <row r="61" spans="7:15">
+      <c r="G61" s="19"/>
+    </row>
+    <row r="62" spans="7:15">
       <c r="G62" s="20"/>
     </row>
-    <row r="63" spans="7:7">
-      <c r="G63" s="19"/>
-    </row>
-    <row r="64" spans="7:7">
+    <row r="63" spans="7:15">
+      <c r="G63" s="20"/>
+    </row>
+    <row r="64" spans="7:15">
       <c r="G64" s="19"/>
     </row>
     <row r="65" spans="2:13">
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="2:13">
-      <c r="F66" s="18"/>
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="2:13">
+      <c r="F67" s="18"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="2:13" customFormat="1">
-      <c r="B68" s="4"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="17"/>
+    <row r="68" spans="2:13">
       <c r="G68" s="19"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="104"/>
-    </row>
-    <row r="69" spans="2:13">
+    </row>
+    <row r="69" spans="2:13" customFormat="1">
+      <c r="B69" s="4"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="17"/>
       <c r="G69" s="19"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="104"/>
     </row>
     <row r="70" spans="2:13">
       <c r="G70" s="19"/>
@@ -6440,23 +6505,32 @@
       <c r="G89" s="19"/>
     </row>
     <row r="90" spans="7:14">
-      <c r="G90" s="20"/>
-      <c r="N90" s="8"/>
+      <c r="G90" s="19"/>
     </row>
     <row r="91" spans="7:14">
-      <c r="G91" s="19"/>
-    </row>
-    <row r="94" spans="7:14">
-      <c r="G94" s="22"/>
+      <c r="G91" s="20"/>
+      <c r="N91" s="8"/>
+    </row>
+    <row r="92" spans="7:14">
+      <c r="G92" s="19"/>
     </row>
     <row r="95" spans="7:14">
-      <c r="G95" s="21"/>
+      <c r="G95" s="22"/>
+    </row>
+    <row r="96" spans="7:14">
+      <c r="G96" s="21"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:M33">
-    <sortCondition ref="B14:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:M34">
+    <sortCondition ref="B14:B34"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
     <mergeCell ref="B12:L12"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -6466,12 +6540,6 @@
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:G8"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" orientation="landscape" r:id="rId1"/>
@@ -6956,23 +7024,23 @@
         <v>66</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -7004,59 +7072,59 @@
     <row r="1" spans="2:9" ht="16" thickBot="1"/>
     <row r="2" spans="2:9">
       <c r="B2" s="59" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F2" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="62" t="s">
         <v>164</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16" thickBot="1">
       <c r="B3" s="63" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F3" s="65" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G3" s="64" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I3" s="66" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C4" s="68">
         <v>7.9000000000000001E-2</v>
@@ -7068,7 +7136,7 @@
         <v>63</v>
       </c>
       <c r="F4" s="71" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G4" s="72">
         <v>8.5999999999999993E-2</v>
@@ -7082,7 +7150,7 @@
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="74" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="55">
         <v>0.11799999999999999</v>
@@ -7094,7 +7162,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G5" s="58">
         <v>0.112</v>
@@ -7108,7 +7176,7 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="74" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C6" s="55">
         <v>0.13800000000000001</v>
@@ -7120,7 +7188,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G6" s="58">
         <v>0.13800000000000001</v>
@@ -7134,7 +7202,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="74" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C7" s="55">
         <v>0.157</v>
@@ -7146,7 +7214,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G7" s="58">
         <v>0.16400000000000001</v>
@@ -7160,7 +7228,7 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C8" s="55">
         <v>0.19700000000000001</v>
@@ -7172,7 +7240,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="54" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G8" s="58">
         <v>0.19</v>
@@ -7186,7 +7254,7 @@
     </row>
     <row r="9" spans="2:9" ht="16" thickBot="1">
       <c r="B9" s="76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C9" s="77">
         <v>0.23599999999999999</v>
@@ -7198,7 +7266,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="80" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G9" s="81">
         <v>0.25</v>
@@ -7212,7 +7280,7 @@
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
@@ -7222,7 +7290,7 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="53" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
@@ -7232,7 +7300,7 @@
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="53" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
@@ -7242,12 +7310,12 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="52" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="52" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>